<commit_message>
pdf copy for invoice 6 created
</commit_message>
<xml_diff>
--- a/Invoices/Invoice Six KCI Cover Sheet.xlsx
+++ b/Invoices/Invoice Six KCI Cover Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CapstoneProject\Invoices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD93EA9B-9215-4B49-9EB7-A8359D66520A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C364F8-DC91-42AA-A6A1-EBE55B9DFC72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -603,10 +603,68 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -638,64 +696,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -936,10 +936,10 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="I1" s="56" t="s">
+      <c r="I1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="37"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:11" ht="15.6">
       <c r="A2" s="1" t="s">
@@ -1072,158 +1072,158 @@
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" thickBot="1"/>
     <row r="12" spans="1:11" thickBot="1">
-      <c r="A12" s="57" t="s">
+      <c r="A12" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="52"/>
-      <c r="C12" s="57" t="s">
+      <c r="B12" s="44"/>
+      <c r="C12" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="58"/>
-      <c r="E12" s="58"/>
-      <c r="F12" s="58"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
       <c r="G12" s="28" t="s">
         <v>19</v>
       </c>
       <c r="H12" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="I12" s="71" t="s">
+      <c r="I12" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="J12" s="72"/>
+      <c r="J12" s="46"/>
     </row>
     <row r="13" spans="1:11" s="32" customFormat="1" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="52"/>
+      <c r="B13" s="44"/>
       <c r="C13" s="53" t="s">
         <v>22</v>
       </c>
       <c r="D13" s="54"/>
       <c r="E13" s="54"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="65">
+      <c r="F13" s="55"/>
+      <c r="G13" s="37">
         <v>35</v>
       </c>
-      <c r="H13" s="64">
+      <c r="H13" s="36">
         <v>1</v>
       </c>
-      <c r="I13" s="75">
+      <c r="I13" s="47">
         <f>G13*H13</f>
         <v>35</v>
       </c>
-      <c r="J13" s="76"/>
+      <c r="J13" s="48"/>
     </row>
     <row r="14" spans="1:11" s="32" customFormat="1" ht="27.75" customHeight="1" thickBot="1">
-      <c r="A14" s="51" t="s">
+      <c r="A14" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="52"/>
+      <c r="B14" s="44"/>
       <c r="C14" s="53" t="s">
         <v>24</v>
       </c>
       <c r="D14" s="54"/>
       <c r="E14" s="54"/>
       <c r="F14" s="54"/>
-      <c r="G14" s="67">
+      <c r="G14" s="39">
         <v>35</v>
       </c>
-      <c r="H14" s="70">
+      <c r="H14" s="40">
         <v>2</v>
       </c>
-      <c r="I14" s="75">
+      <c r="I14" s="47">
         <f t="shared" ref="I14" si="0">G14*H14</f>
         <v>70</v>
       </c>
-      <c r="J14" s="76"/>
+      <c r="J14" s="48"/>
     </row>
     <row r="15" spans="1:11" s="32" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A15" s="51" t="s">
+      <c r="A15" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="52"/>
+      <c r="B15" s="44"/>
       <c r="C15" s="53" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="54"/>
       <c r="E15" s="54"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="66">
+      <c r="F15" s="55"/>
+      <c r="G15" s="38">
         <v>35</v>
       </c>
-      <c r="H15" s="64">
+      <c r="H15" s="36">
         <v>0.5</v>
       </c>
-      <c r="I15" s="73">
+      <c r="I15" s="56">
         <f>G15*H15</f>
         <v>17.5</v>
       </c>
-      <c r="J15" s="74"/>
+      <c r="J15" s="57"/>
     </row>
     <row r="16" spans="1:11" s="32" customFormat="1" thickBot="1">
-      <c r="A16" s="55"/>
-      <c r="B16" s="60"/>
-      <c r="C16" s="61"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="63"/>
+      <c r="A16" s="58"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="62"/>
       <c r="G16" s="35"/>
       <c r="H16" s="35"/>
-      <c r="I16" s="68"/>
-      <c r="J16" s="69"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="51"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A17" s="48"/>
-      <c r="B17" s="47"/>
-      <c r="C17" s="50" t="s">
+      <c r="A17" s="74"/>
+      <c r="B17" s="73"/>
+      <c r="C17" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
       <c r="H17" s="29"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="43"/>
+      <c r="I17" s="68"/>
+      <c r="J17" s="69"/>
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A18" s="48"/>
-      <c r="B18" s="47"/>
-      <c r="C18" s="44" t="s">
+      <c r="A18" s="74"/>
+      <c r="B18" s="73"/>
+      <c r="C18" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="46">
+      <c r="D18" s="71"/>
+      <c r="E18" s="71"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="71"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="72">
         <f>SUM(I13:I17)</f>
         <v>122.5</v>
       </c>
-      <c r="J18" s="47"/>
+      <c r="J18" s="73"/>
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A19" s="49"/>
-      <c r="B19" s="37"/>
+      <c r="A19" s="75"/>
+      <c r="B19" s="42"/>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A20" s="39"/>
-      <c r="B20" s="40"/>
+      <c r="A20" s="65"/>
+      <c r="B20" s="66"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A21" s="41"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="37"/>
+      <c r="A21" s="67"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="63"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="64"/>
+      <c r="J21" s="42"/>
       <c r="K21" s="4"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1">
@@ -2209,22 +2209,6 @@
     <row r="978" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
     <mergeCell ref="C21:H21"/>
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="A20:B20"/>
@@ -2236,6 +2220,22 @@
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="C17:G17"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="C12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>